<commit_message>
Atualização do Product Backlog e Requisitos adicionados na Documentação
</commit_message>
<xml_diff>
--- a/Arquivos/Product e Sprint Backlog.xlsx
+++ b/Arquivos/Product e Sprint Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/emmily_jesus_sptech_school/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9aaeaea6ef72b91c/Documentos/Repositórios de Projetos/Projeto_TechSolutions/Projeto-TechSolutions/Arquivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4088" documentId="8_{A18475A0-CC0B-4C0F-A858-D681464BEF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C74C5000-55F2-4A84-A581-437E72791908}"/>
+  <xr:revisionPtr revIDLastSave="4097" documentId="8_{A18475A0-CC0B-4C0F-A858-D681464BEF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD183ED4-1E31-485F-AABD-5A7BB4C68C22}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="511" xr2:uid="{CF0E2B86-90F2-4F48-8623-DE82AABC8440}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="187">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -579,9 +579,6 @@
     <t>Atualização de arquivos e membros no repositório do GitHub, e alterações da Documentação.</t>
   </si>
   <si>
-    <t>O Protótipo do Menu de navegação na vertical deve ter conter um conjunto de links e icones: Icone de usuário com frase "Bem Vindo", logo abaixo Perfil, Dashboard, Armazém, Funcionários e Botão Sair. O link deve ficar em negrito conforme estiver na página selecionada.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Importante</t>
   </si>
   <si>
@@ -589,6 +586,18 @@
   </si>
   <si>
     <t>Diagrama que representa a solução proposta.</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Menu de navegação na vertical deve conter um conjunto de links e icones: Icone de usuário com frase "Bem Vindo", logo abaixo Perfil, Dashboard, Armazém e Funcionários. O link deve ficar em negrito conforme estiver na página selecionada.</t>
+  </si>
+  <si>
+    <t>O Protótipo do Menu de navegação na vertical deve conter um conjunto de links e icones: Icone de usuário com frase "Bem Vindo", logo abaixo Perfil, Dashboard, Armazém, Funcionários e Botão Sair. O link deve ficar em negrito conforme estiver na página selecionada.</t>
+  </si>
+  <si>
+    <t>A tela Dashboard deve conter gráfico em linhas com variações da umidade e do horário de cada armazem, e um gráfico em pizza apresentando a quantidade de alertas em vermelho, laranja e amarelo.  Desenvolvimento da Tela da Dashboard em HTML e CSS</t>
   </si>
 </sst>
 </file>
@@ -900,9 +909,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -930,6 +936,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2210,10 +2219,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:K82"/>
+  <dimension ref="A2:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2228,39 +2237,39 @@
     <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-    </row>
-    <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-    </row>
-    <row r="5" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
@@ -2312,8 +2321,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+    <row r="7" spans="1:12" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
       <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
@@ -2339,7 +2348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2364,8 +2373,11 @@
       <c r="I8" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2420,7 +2432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2446,7 +2458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -2550,7 +2562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -2610,7 +2622,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>46</v>
@@ -2636,7 +2648,7 @@
         <v>176</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>12</v>
@@ -2992,29 +3004,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="21" t="s">
+    <row r="33" spans="2:11" s="24" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="23" t="s">
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="1">
         <v>3</v>
       </c>
-      <c r="H33" s="23">
-        <v>1</v>
-      </c>
-      <c r="I33" s="21" t="s">
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="12" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3263,7 +3275,7 @@
         <v>96</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>12</v>
@@ -3809,7 +3821,7 @@
         <v>136</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>17</v>
@@ -4332,36 +4344,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
@@ -4397,7 +4409,7 @@
         <v>45</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>46</v>
@@ -4416,7 +4428,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
@@ -4583,10 +4595,10 @@
         <v>136</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>44</v>

</xml_diff>